<commit_message>
cleaned up the code a lil bit
</commit_message>
<xml_diff>
--- a/files/movies.xlsx
+++ b/files/movies.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tmdb_webscraper\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Movie</t>
   </si>
@@ -35,13 +40,24 @@
   </si>
   <si>
     <t>Beyond the Dream</t>
+  </si>
+  <si>
+    <t>Dune</t>
+  </si>
+  <si>
+    <t>The Shawshank Redemption</t>
+  </si>
+  <si>
+    <t>Howl's Moving Castle</t>
+  </si>
+  <si>
+    <t>The Wind Rises</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,25 +101,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -114,10 +133,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -155,71 +174,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -247,7 +266,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -270,11 +289,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -283,13 +302,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -299,7 +318,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -308,7 +327,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -317,7 +336,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -325,10 +344,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -397,48 +416,70 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="3" width="31.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="31.109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="4" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>